<commit_message>
add first draft csic irregular
</commit_message>
<xml_diff>
--- a/data/csic-irregular/csic-irregular-terrains.xlsx
+++ b/data/csic-irregular/csic-irregular-terrains.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="152">
   <si>
     <t xml:space="preserve">Scenario-Protocol-PI-PI Algo template</t>
   </si>
@@ -99,7 +99,7 @@
     <t xml:space="preserve">Suitable Bipedal Systems</t>
   </si>
   <si>
-    <t xml:space="preserve">Human, Prosthesis, Exosqueleton</t>
+    <t xml:space="preserve">Human, Prosthesis, Exoskeleton</t>
   </si>
   <si>
     <t xml:space="preserve">Possible values: Humanoid, prosthesis, exoskeleton, human</t>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">Associated PI Algo</t>
   </si>
   <si>
-    <t xml:space="preserve">margin_stability, ratioIndex, variability, walkRatio</t>
+    <t xml:space="preserve">margin_stability, ratio_index, variability, walk_ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Estimated experimentation duration</t>
@@ -156,10 +156,10 @@
     <t xml:space="preserve">Technical File Sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">Optoelectronic motion capture system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VICON</t>
+    <t xml:space="preserve">Optoelectronic motion capture system or Vicon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensor</t>
   </si>
   <si>
     <t xml:space="preserve">https://docs.vicon.com/display/Nexus210</t>
@@ -177,19 +177,16 @@
     <t xml:space="preserve">EMG+IMU sensors</t>
   </si>
   <si>
-    <t xml:space="preserve">DELSYS (Trigno Avanti)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://delsys.com/trigno/research/#trigno-avanti-sensor</t>
+    <t xml:space="preserve">DELSYS (Trigno Avanti) https://delsys.com/trigno/research/#trigno-avanti-sensor </t>
   </si>
   <si>
     <t xml:space="preserve">Sensorized insoles</t>
   </si>
   <si>
-    <t xml:space="preserve">MOTICON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.moticon.de/insole3-specs/</t>
+    <t xml:space="preserve">MOTICON https://www.moticon.de/insole3-specs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipment</t>
   </si>
   <si>
     <t xml:space="preserve">3x1m commercial platform (PARALELA PLUS from Chinesport) with a fixed wooden board with holes into which anti-slip 50x50cm wooden modules, terrasensa modules or mats can be fitted. </t>
@@ -204,7 +201,7 @@
     <t xml:space="preserve">Complementary information</t>
   </si>
   <si>
-    <t xml:space="preserve">Place the optical markers onto the subject's body and take the required anthropometric measurements.</t>
+    <t xml:space="preserve">Place the optical markers and Delsys sensors onto the subject's body and take the required anthropometric measurements. Place the sensorized insoles in the subjects' shoes.</t>
   </si>
   <si>
     <t xml:space="preserve">Following the VICON's "Full Body Plug in Gait" marker set specifications (https://docs.vicon.com/display/Nexus26/Full+body+modeling+with+Plug-in+Gait) and  adding 8 clusters (thighs, tibias, feet, pelvis, chest).</t>
@@ -269,7 +266,7 @@
     <t xml:space="preserve">Margin of Stability (MoS)</t>
   </si>
   <si>
-    <t xml:space="preserve">Analogous parameter to the condition of standing stability which states that the center of mass (CoM) should be within the base of support (BoS). The extrapolation to dynamic stability states that the position of the vertical projection of the CoM (PCoM) plus its velocity times a factor (extrapolated center of mass position (XCoM)) should be within the BoS.</t>
+    <t xml:space="preserve">Analogous parameter to the condition of standing stability which states that the center of mass (CoM) should be within the base of support (BoS). The extrapolation to dynamic stability states that the position of the vertical projection of the CoM (PCoM) plus its velocity times a factor (extrapolated center of mass position (XCoM)) should be within the BoS. </t>
   </si>
   <si>
     <t xml:space="preserve">cm</t>
@@ -296,36 +293,39 @@
     <t xml:space="preserve">Gait Deviation Index (GDI)</t>
   </si>
   <si>
-    <t xml:space="preserve">Scaled distance between 15 gait feature scores for a subject and the average of the same 15 gait feature scores for a control group of typically developing (TD) children.</t>
+    <t xml:space="preserve">Scaled distance between 15 gait feature scores for a subject and the average of the same 15 gait feature scores for a control group of typically developing (TD) children. </t>
   </si>
   <si>
     <t xml:space="preserve">- </t>
   </si>
   <si>
+    <t xml:space="preserve">Walk Ratio (WR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division of step length by cadence. It is used to measure overall gait control.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm/(step/min)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gait Parameters Variability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference between the value of a gait parameter when walking without the exoskeleton and the value of the same gait parameter obtained when walking wearing the exoskeleton.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit of the gait parameter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scalar</t>
   </si>
   <si>
-    <t xml:space="preserve">Walk Ratio (WR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Division of step length by cadence. It is used to measure overall gait control.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm/(step/min)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gait Parameters Variability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difference between the value of a gait parameter when walking without the exoskeleton and the value of the same gait parameter obtained when walking wearing the exoskeleton.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit of the gait parameter</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ratio Index (RI)</t>
   </si>
   <si>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">Input command</t>
   </si>
   <si>
-    <t xml:space="preserve">"./run_pi;GaitEvents.csv;Anthropometry.yaml;com.csv;FeetTrajectories.csv"</t>
+    <t xml:space="preserve">[ ./run_pi_margin_stability, COM_plano01.csv, gaitEvents_plano01.csv, FeetTrajectories_plano01.csv, Anthropometry.yaml]</t>
   </si>
   <si>
     <t xml:space="preserve">Additional information on the code development (just needed for checking advancement)</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Operating System</t>
   </si>
   <si>
-    <t xml:space="preserve">macOS Catalina 10.15.2</t>
+    <t xml:space="preserve">Windows 10</t>
   </si>
   <si>
     <t xml:space="preserve">Version Control System</t>
@@ -437,7 +437,7 @@
     <t xml:space="preserve">https://github.com/AdrianaTorres/Irregular_Terrains/tree/master/Walk_Ratio_octave</t>
   </si>
   <si>
-    <t xml:space="preserve">[walking_ratio]</t>
+    <t xml:space="preserve">[walk_ratio]</t>
   </si>
   <si>
     <t xml:space="preserve">gaitParameters.yaml</t>
@@ -446,7 +446,7 @@
     <t xml:space="preserve">Input files should be included in the data format</t>
   </si>
   <si>
-    <t xml:space="preserve">"./run_pi;gaitParameters.yaml"</t>
+    <t xml:space="preserve">[./run_pi_walk_ratio, GaitParameters_noExo.yaml]</t>
   </si>
   <si>
     <t xml:space="preserve">variability</t>
@@ -461,6 +461,9 @@
     <t xml:space="preserve">[gait_parameters_variability]</t>
   </si>
   <si>
+    <t xml:space="preserve">[./run_pi_variability, GaitParameters_exo.yaml, GaitParameters_noExo.yaml]</t>
+  </si>
+  <si>
     <t xml:space="preserve">ratioIndex</t>
   </si>
   <si>
@@ -474,6 +477,9 @@
   </si>
   <si>
     <t xml:space="preserve">[ratio_index]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[./run_pi_ratio_index, GaitParameters_noExo.yaml]</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -556,8 +562,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -576,7 +595,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,6 +612,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5B9BD5"/>
         <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -707,7 +732,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -800,6 +825,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -808,6 +837,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -816,6 +853,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -908,12 +949,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -928,15 +985,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,7 +1029,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1039,9 +1096,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1895040</xdr:colOff>
+      <xdr:colOff>1894680</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2676240</xdr:rowOff>
+      <xdr:rowOff>2675880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1055,7 +1112,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2312640" y="1304640"/>
-          <a:ext cx="1895040" cy="2676240"/>
+          <a:ext cx="1894680" cy="2675880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1076,9 +1133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1895040</xdr:colOff>
+      <xdr:colOff>1894680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>894960</xdr:rowOff>
+      <xdr:rowOff>894600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1092,7 +1149,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2312640" y="6467400"/>
-          <a:ext cx="1895040" cy="894960"/>
+          <a:ext cx="1894680" cy="894600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1113,9 +1170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>132480</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>199800</xdr:rowOff>
+      <xdr:rowOff>199440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1128,8 +1185,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4238280" y="14811120"/>
-          <a:ext cx="132840" cy="199800"/>
+          <a:off x="4238280" y="14801760"/>
+          <a:ext cx="132480" cy="199440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2506,8 +2563,8 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2779,17 +2836,17 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="21"/>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="21"/>
@@ -2811,9 +2868,9 @@
         <v>48</v>
       </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="21"/>
@@ -2834,56 +2891,58 @@
       <c r="B31" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="21"/>
       <c r="B32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="21"/>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
+      <c r="C33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="C34" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="21"/>
@@ -2891,13 +2950,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="21"/>
@@ -2905,13 +2964,13 @@
         <v>2</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="21"/>
@@ -2919,25 +2978,25 @@
         <v>3</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+        <v>63</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="21"/>
       <c r="B38" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="21"/>
@@ -2945,25 +3004,25 @@
         <v>5</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
+        <v>66</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="21"/>
       <c r="B40" s="18" t="n">
         <v>6</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="21"/>
@@ -2971,13 +3030,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="21"/>
@@ -2985,11 +3044,11 @@
         <v>8</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="21"/>
@@ -2997,11 +3056,11 @@
         <v>9</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+        <v>72</v>
+      </c>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="21"/>
@@ -3009,11 +3068,11 @@
         <v>10</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
+        <v>73</v>
+      </c>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="21"/>
@@ -3021,11 +3080,11 @@
         <v>11</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
+        <v>74</v>
+      </c>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="21"/>
@@ -3033,11 +3092,11 @@
         <v>12</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
+        <v>75</v>
+      </c>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4068,8 +4127,8 @@
   </sheetPr>
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G128" activeCellId="0" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4082,13 +4141,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="8"/>
     </row>
@@ -4102,18 +4161,18 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="20" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,34 +4180,34 @@
         <v>34</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>87</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4161,251 +4220,251 @@
       <c r="B12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" s="38" t="s">
+      <c r="A14" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="11" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="42" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="38" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>91</v>
+      <c r="A18" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="38" t="s">
+      <c r="A23" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="42" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="20" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="42" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="38" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="42" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="42" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="40" t="s">
+      <c r="B37" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B40" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="33" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B42" s="48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="37" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="37" t="s">
+      <c r="D46" s="38" t="s">
         <v>87</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46" s="34" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4415,14 +4474,14 @@
       <c r="B49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="45"/>
+      <c r="B50" s="49"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="46"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="51"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
@@ -4452,7 +4511,7 @@
       <c r="A55" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="48" t="s">
+      <c r="B55" s="52" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4460,7 +4519,7 @@
       <c r="A56" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="49" t="s">
+      <c r="B56" s="53" t="s">
         <v>110</v>
       </c>
     </row>
@@ -4482,10 +4541,10 @@
       <c r="A59" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="50" t="s">
+      <c r="B59" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="38" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4493,7 +4552,7 @@
       <c r="A60" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="55" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4521,7 +4580,7 @@
       <c r="A66" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="42" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4529,7 +4588,7 @@
       <c r="A67" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="56" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4572,14 +4631,14 @@
       <c r="B74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B75" s="45"/>
+      <c r="B75" s="49"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="46"/>
-      <c r="B76" s="47"/>
+      <c r="A76" s="50"/>
+      <c r="B76" s="51"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="15" t="s">
@@ -4593,7 +4652,7 @@
       <c r="A78" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B78" s="51" t="s">
+      <c r="B78" s="57" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4606,10 +4665,10 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="33" t="s">
+      <c r="A80" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B80" s="49" t="s">
+      <c r="B80" s="53" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4617,7 +4676,7 @@
       <c r="A81" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="49" t="s">
+      <c r="B81" s="53" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4642,7 +4701,7 @@
       <c r="B84" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D84" s="34" t="s">
+      <c r="D84" s="38" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4650,7 +4709,7 @@
       <c r="A85" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="58" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4678,7 +4737,7 @@
       <c r="A91" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B91" s="38" t="s">
+      <c r="B91" s="42" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4686,7 +4745,7 @@
       <c r="A92" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="56" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4729,14 +4788,14 @@
       <c r="B99" s="7"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="45" t="s">
+      <c r="A100" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="45"/>
+      <c r="B100" s="49"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="46"/>
-      <c r="B101" s="47"/>
+      <c r="A101" s="50"/>
+      <c r="B101" s="51"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="15" t="s">
@@ -4755,7 +4814,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="33" t="s">
+      <c r="A104" s="37" t="s">
         <v>10</v>
       </c>
       <c r="B104" s="11" t="s">
@@ -4763,18 +4822,18 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="33" t="s">
+      <c r="A105" s="37" t="s">
         <v>107</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="49" t="s">
+      <c r="B106" s="53" t="s">
         <v>143</v>
       </c>
     </row>
@@ -4799,7 +4858,7 @@
       <c r="B109" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D109" s="34" t="s">
+      <c r="D109" s="38" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4807,8 +4866,8 @@
       <c r="A110" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="20" t="s">
-        <v>140</v>
+      <c r="B110" s="59" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4835,7 +4894,7 @@
       <c r="A116" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B116" s="38" t="s">
+      <c r="B116" s="42" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4843,7 +4902,7 @@
       <c r="A117" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="B117" s="56" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4880,167 +4939,167 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="52" t="s">
+      <c r="A124" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="B124" s="52"/>
+      <c r="B124" s="60"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="53" t="s">
+      <c r="A125" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="B125" s="53"/>
+      <c r="B125" s="61"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="54"/>
-      <c r="B126" s="38"/>
+      <c r="A126" s="62"/>
+      <c r="B126" s="42"/>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="40" t="s">
+      <c r="A127" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B127" s="41" t="s">
+      <c r="B127" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="37" t="s">
+      <c r="A128" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B128" s="55" t="s">
-        <v>145</v>
+      <c r="B128" s="63" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="37" t="s">
+      <c r="A129" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B129" s="38" t="s">
-        <v>146</v>
+      <c r="B129" s="42" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="37" t="s">
+      <c r="A130" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B130" s="56" t="s">
-        <v>147</v>
+      <c r="B130" s="64" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="37" t="s">
+      <c r="A131" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B131" s="57" t="s">
-        <v>148</v>
+      <c r="B131" s="65" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B132" s="38"/>
+      <c r="B132" s="42"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="37" t="s">
+      <c r="A133" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B133" s="58" t="s">
-        <v>149</v>
+      <c r="B133" s="66" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="37" t="s">
+      <c r="A134" s="41" t="s">
         <v>114</v>
       </c>
       <c r="B134" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D134" s="34" t="s">
+      <c r="D134" s="38" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="37" t="s">
+      <c r="A135" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="B135" s="20" t="s">
-        <v>140</v>
+      <c r="B135" s="59" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="34"/>
-      <c r="B136" s="34"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="38"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="59" t="s">
+      <c r="A137" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="B137" s="59"/>
+      <c r="B137" s="67"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="59" t="s">
+      <c r="A138" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="B138" s="59"/>
+      <c r="B138" s="67"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="60"/>
-      <c r="B139" s="60"/>
+      <c r="A139" s="68"/>
+      <c r="B139" s="68"/>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="40" t="s">
+      <c r="A140" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B140" s="41" t="s">
+      <c r="B140" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="37" t="s">
+      <c r="A141" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="B141" s="38" t="s">
+      <c r="B141" s="42" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="37" t="s">
+      <c r="A142" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B142" s="38" t="s">
+      <c r="B142" s="56" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="37" t="s">
+      <c r="A143" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B143" s="38" t="s">
+      <c r="B143" s="42" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="37" t="s">
+      <c r="A144" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="B144" s="38" t="s">
+      <c r="B144" s="42" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="61" t="s">
+      <c r="A145" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="B145" s="38" t="s">
+      <c r="B145" s="42" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="37" t="s">
+      <c r="A146" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="B146" s="38" t="s">
+      <c r="B146" s="42" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>